<commit_message>
Handle Ke Dien Tu
</commit_message>
<xml_diff>
--- a/adg-api/src/main/resources/2. Kê Điện Tử.xlsx
+++ b/adg-api/src/main/resources/2. Kê Điện Tử.xlsx
@@ -61,7 +61,7 @@
     <t>Công ty chúng tôi cam kết</t>
   </si>
   <si>
-    <t>+      Các chứng từ điện tử đã kê khai đề nghị giải ngân là hợp pháp, hợp lệ.</t>
+    <t>+     Các chứng từ điện tử đã kê khai đề nghị giải ngân là hợp pháp, hợp lệ.</t>
   </si>
   <si>
     <t>+     Công ty chúng tôi chưa vay vốn tại bất kỳ TCTD nào để thanh toán cho các chứng từ điện tử được kê khai đề nghị giải ngân.</t>
@@ -80,6 +80,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0[$ ₫]"/>
+  </numFmts>
   <fonts count="8">
     <font>
       <sz val="10.0"/>
@@ -172,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -189,6 +192,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -199,6 +205,9 @@
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -215,7 +224,7 @@
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
@@ -491,69 +500,69 @@
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6" t="s">
+      <c r="D10" s="6"/>
+      <c r="E10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8" t="s">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
     </row>
     <row r="13">
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
     </row>
     <row r="14">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17">
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18">
-      <c r="D18" s="15" t="s">
+    <row r="18" ht="23.25" customHeight="1">
+      <c r="D18" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19">
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="18" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:F14"/>
     <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B14:F14"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:F3"/>
     <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:F4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D3:F3"/>
     <mergeCell ref="A8:F8"/>
     <mergeCell ref="B11:C11"/>
   </mergeCells>

</xml_diff>